<commit_message>
w3d3 exercise and xlsx output file
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -7,10 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Characters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Locations" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Episodes" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Characters" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Locations" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rick and Morty Episodes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,22 +461,4 @@
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
w3d3 exercise - headers created
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -415,14 +415,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>info</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>results</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
w3d3 damn it :(
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,53 +434,6 @@
           <t>results</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>r</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>u</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>l</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>t</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
w3d3 - headers for single character
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,12 +426,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>info</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>results</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>gender</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>origin</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>location</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>episode</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>created</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
w3d3 - ok, getting some new info.
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,62 +426,744 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>species</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>type</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>gender</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>origin</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>image</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>episode</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>url</t>
+          <t>('id', 6)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>created</t>
+          <t>('id', 6)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>('name', 'Abadango Cluster Princess')</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>('status', 'Alive')</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>('species', 'Alien')</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>('type', '')</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>('gender', 'Female')</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>('origin', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>('location', {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'})</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>('image', 'https://rickandmortyapi.com/api/character/avatar/6.jpeg')</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>('episode', ['https://rickandmortyapi.com/api/episode/27'])</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>('url', 'https://rickandmortyapi.com/api/character/6')</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>('created', '2017-11-04T19:50:28.250Z')</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
w3d3 - not quite. just need the RESULTS
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -488,58 +488,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>('info', {'count': 826, 'pages': 42, 'next': 'https://rickandmortyapi.com/api/character?page=2', 'prev': None})</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Abadango Cluster Princess</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Alien</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>{'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>https://rickandmortyapi.com/api/character/avatar/6.jpeg</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>['https://rickandmortyapi.com/api/episode/27']</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>https://rickandmortyapi.com/api/character/6</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2017-11-04T19:50:28.250Z</t>
+          <t>('results', [{'id': 1, 'name': 'Rick Sanchez', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/1.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/1', 'created': '2017-11-04T18:48:46.250Z'}, {'id': 2, 'name': 'Morty Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/2.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/2', 'created': '2017-11-04T18:50:21.651Z'}, {'id': 3, 'name': 'Summer Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/3.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/3', 'created': '2017-11-04T19:09:56.428Z'}, {'id': 4, 'name': 'Beth Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/4.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/4', 'created': '2017-11-04T19:22:43.665Z'}, {'id': 5, 'name': 'Jerry Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/5.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/5', 'created': '2017-11-04T19:26:56.301Z'}, {'id': 6, 'name': 'Abadango Cluster Princess', 'status': 'Alive', 'species': 'Alien', 'type': '', 'gender': 'Female', 'origin': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'location': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/6.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/27'], 'url': 'https://rickandmortyapi.com/api/character/6', 'created': '2017-11-04T19:50:28.250Z'}, {'id': 7, 'name': 'Abradolf Lincler', 'status': 'unknown', 'species': 'Human', 'type': 'Genetic experiment', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Testicle Monster Dimension', 'url': 'https://rickandmortyapi.com/api/location/21'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/7.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11'], 'url': 'https://rickandmortyapi.com/api/character/7', 'created': '2017-11-04T19:59:20.523Z'}, {'id': 8, 'name': 'Adjudicator Rick', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/8.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/8', 'created': '2017-11-04T20:03:34.737Z'}, {'id': 9, 'name': 'Agency Director', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/9.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/24'], 'url': 'https://rickandmortyapi.com/api/character/9', 'created': '2017-11-04T20:06:54.976Z'}, {'id': 10, 'name': 'Alan Rails', 'status': 'Dead', 'species': 'Human', 'type': 'Superhuman (Ghost trains summoner)', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': "Worldender's lair", 'url': 'https://rickandmortyapi.com/api/location/4'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/10.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/25'], 'url': 'https://rickandmortyapi.com/api/character/10', 'created': '2017-11-04T20:19:09.017Z'}, {'id': 11, 'name': 'Albert Einstein', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/11.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/12'], 'url': 'https://rickandmortyapi.com/api/character/11', 'created': '2017-11-04T20:20:20.965Z'}, {'id': 12, 'name': 'Alexander', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/12.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/12', 'created': '2017-11-04T20:32:33.144Z'}, {'id': 13, 'name': 'Alien Googah', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'unknown', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/13.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/31'], 'url': 'https://rickandmortyapi.com/api/character/13', 'created': '2017-11-04T20:33:30.779Z'}, {'id': 14, 'name': 'Alien Morty', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/14.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/14', 'created': '2017-11-04T20:51:31.373Z'}, {'id': 15, 'name': 'Alien Rick', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/15.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/15', 'created': '2017-11-04T20:56:13.215Z'}, {'id': 16, 'name': 'Amish Cyborg', 'status': 'Dead', 'species': 'Alien', 'type': 'Parasite', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/16.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/15'], 'url': 'https://rickandmortyapi.com/api/character/16', 'created': '2017-11-04T21:12:45.235Z'}, {'id': 17, 'name': 'Annie', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/17.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/17', 'created': '2017-11-04T22:21:24.481Z'}, {'id': 18, 'name': 'Antenna Morty', 'status': 'Alive', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/18.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/18', 'created': '2017-11-04T22:25:29.008Z'}, {'id': 19, 'name': 'Antenna Rick', 'status': 'unknown', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'unknown', 'url': ''}, 'image': 'https://rickandmortyapi.com/api/character/avatar/19.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/19', 'created': '2017-11-04T22:28:13.756Z'}, {'id': 20, 'name': 'Ants in my Eyes Johnson', 'status': 'unknown', 'species': 'Human', 'type': 'Human with ants in his eyes', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Interdimensional Cable', 'url': 'https://rickandmortyapi.com/api/location/6'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/20.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/8'], 'url': 'https://rickandmortyapi.com/api/character/20', 'created': '2017-11-04T22:34:53.659Z'}])</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
w3d3 - still not right
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d3_exercise.xlsx
+++ b/week_3/spreadsheets/w3_d3_exercise.xlsx
@@ -488,12 +488,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>('info', {'count': 826, 'pages': 42, 'next': 'https://rickandmortyapi.com/api/character?page=2', 'prev': None})</t>
+          <t>{'count': 826, 'pages': 42, 'next': 'https://rickandmortyapi.com/api/character?page=2', 'prev': None}</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('results', [{'id': 1, 'name': 'Rick Sanchez', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/1.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/1', 'created': '2017-11-04T18:48:46.250Z'}, {'id': 2, 'name': 'Morty Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/2.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/2', 'created': '2017-11-04T18:50:21.651Z'}, {'id': 3, 'name': 'Summer Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/3.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/3', 'created': '2017-11-04T19:09:56.428Z'}, {'id': 4, 'name': 'Beth Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/4.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/4', 'created': '2017-11-04T19:22:43.665Z'}, {'id': 5, 'name': 'Jerry Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/5.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/5', 'created': '2017-11-04T19:26:56.301Z'}, {'id': 6, 'name': 'Abadango Cluster Princess', 'status': 'Alive', 'species': 'Alien', 'type': '', 'gender': 'Female', 'origin': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'location': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/6.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/27'], 'url': 'https://rickandmortyapi.com/api/character/6', 'created': '2017-11-04T19:50:28.250Z'}, {'id': 7, 'name': 'Abradolf Lincler', 'status': 'unknown', 'species': 'Human', 'type': 'Genetic experiment', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Testicle Monster Dimension', 'url': 'https://rickandmortyapi.com/api/location/21'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/7.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11'], 'url': 'https://rickandmortyapi.com/api/character/7', 'created': '2017-11-04T19:59:20.523Z'}, {'id': 8, 'name': 'Adjudicator Rick', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/8.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/8', 'created': '2017-11-04T20:03:34.737Z'}, {'id': 9, 'name': 'Agency Director', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/9.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/24'], 'url': 'https://rickandmortyapi.com/api/character/9', 'created': '2017-11-04T20:06:54.976Z'}, {'id': 10, 'name': 'Alan Rails', 'status': 'Dead', 'species': 'Human', 'type': 'Superhuman (Ghost trains summoner)', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': "Worldender's lair", 'url': 'https://rickandmortyapi.com/api/location/4'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/10.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/25'], 'url': 'https://rickandmortyapi.com/api/character/10', 'created': '2017-11-04T20:19:09.017Z'}, {'id': 11, 'name': 'Albert Einstein', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/11.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/12'], 'url': 'https://rickandmortyapi.com/api/character/11', 'created': '2017-11-04T20:20:20.965Z'}, {'id': 12, 'name': 'Alexander', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/12.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/12', 'created': '2017-11-04T20:32:33.144Z'}, {'id': 13, 'name': 'Alien Googah', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'unknown', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/13.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/31'], 'url': 'https://rickandmortyapi.com/api/character/13', 'created': '2017-11-04T20:33:30.779Z'}, {'id': 14, 'name': 'Alien Morty', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/14.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/14', 'created': '2017-11-04T20:51:31.373Z'}, {'id': 15, 'name': 'Alien Rick', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/15.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/15', 'created': '2017-11-04T20:56:13.215Z'}, {'id': 16, 'name': 'Amish Cyborg', 'status': 'Dead', 'species': 'Alien', 'type': 'Parasite', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/16.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/15'], 'url': 'https://rickandmortyapi.com/api/character/16', 'created': '2017-11-04T21:12:45.235Z'}, {'id': 17, 'name': 'Annie', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/17.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/17', 'created': '2017-11-04T22:21:24.481Z'}, {'id': 18, 'name': 'Antenna Morty', 'status': 'Alive', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/18.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/18', 'created': '2017-11-04T22:25:29.008Z'}, {'id': 19, 'name': 'Antenna Rick', 'status': 'unknown', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'unknown', 'url': ''}, 'image': 'https://rickandmortyapi.com/api/character/avatar/19.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/19', 'created': '2017-11-04T22:28:13.756Z'}, {'id': 20, 'name': 'Ants in my Eyes Johnson', 'status': 'unknown', 'species': 'Human', 'type': 'Human with ants in his eyes', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Interdimensional Cable', 'url': 'https://rickandmortyapi.com/api/location/6'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/20.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/8'], 'url': 'https://rickandmortyapi.com/api/character/20', 'created': '2017-11-04T22:34:53.659Z'}])</t>
+          <t>[{'id': 1, 'name': 'Rick Sanchez', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/1.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/1', 'created': '2017-11-04T18:48:46.250Z'}, {'id': 2, 'name': 'Morty Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/2.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/1', 'https://rickandmortyapi.com/api/episode/2', 'https://rickandmortyapi.com/api/episode/3', 'https://rickandmortyapi.com/api/episode/4', 'https://rickandmortyapi.com/api/episode/5', 'https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/37', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/2', 'created': '2017-11-04T18:50:21.651Z'}, {'id': 3, 'name': 'Summer Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/3.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/17', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/3', 'created': '2017-11-04T19:09:56.428Z'}, {'id': 4, 'name': 'Beth Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/4.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/24', 'https://rickandmortyapi.com/api/episode/25', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/27', 'https://rickandmortyapi.com/api/episode/28', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/34', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/4', 'created': '2017-11-04T19:22:43.665Z'}, {'id': 5, 'name': 'Jerry Smith', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/5.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/6', 'https://rickandmortyapi.com/api/episode/7', 'https://rickandmortyapi.com/api/episode/8', 'https://rickandmortyapi.com/api/episode/9', 'https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11', 'https://rickandmortyapi.com/api/episode/12', 'https://rickandmortyapi.com/api/episode/13', 'https://rickandmortyapi.com/api/episode/14', 'https://rickandmortyapi.com/api/episode/15', 'https://rickandmortyapi.com/api/episode/16', 'https://rickandmortyapi.com/api/episode/18', 'https://rickandmortyapi.com/api/episode/19', 'https://rickandmortyapi.com/api/episode/20', 'https://rickandmortyapi.com/api/episode/21', 'https://rickandmortyapi.com/api/episode/22', 'https://rickandmortyapi.com/api/episode/23', 'https://rickandmortyapi.com/api/episode/26', 'https://rickandmortyapi.com/api/episode/29', 'https://rickandmortyapi.com/api/episode/30', 'https://rickandmortyapi.com/api/episode/31', 'https://rickandmortyapi.com/api/episode/32', 'https://rickandmortyapi.com/api/episode/33', 'https://rickandmortyapi.com/api/episode/35', 'https://rickandmortyapi.com/api/episode/36', 'https://rickandmortyapi.com/api/episode/38', 'https://rickandmortyapi.com/api/episode/39', 'https://rickandmortyapi.com/api/episode/40', 'https://rickandmortyapi.com/api/episode/41', 'https://rickandmortyapi.com/api/episode/42', 'https://rickandmortyapi.com/api/episode/43', 'https://rickandmortyapi.com/api/episode/44', 'https://rickandmortyapi.com/api/episode/45', 'https://rickandmortyapi.com/api/episode/46', 'https://rickandmortyapi.com/api/episode/47', 'https://rickandmortyapi.com/api/episode/48', 'https://rickandmortyapi.com/api/episode/49', 'https://rickandmortyapi.com/api/episode/50', 'https://rickandmortyapi.com/api/episode/51'], 'url': 'https://rickandmortyapi.com/api/character/5', 'created': '2017-11-04T19:26:56.301Z'}, {'id': 6, 'name': 'Abadango Cluster Princess', 'status': 'Alive', 'species': 'Alien', 'type': '', 'gender': 'Female', 'origin': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'location': {'name': 'Abadango', 'url': 'https://rickandmortyapi.com/api/location/2'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/6.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/27'], 'url': 'https://rickandmortyapi.com/api/character/6', 'created': '2017-11-04T19:50:28.250Z'}, {'id': 7, 'name': 'Abradolf Lincler', 'status': 'unknown', 'species': 'Human', 'type': 'Genetic experiment', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Testicle Monster Dimension', 'url': 'https://rickandmortyapi.com/api/location/21'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/7.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/11'], 'url': 'https://rickandmortyapi.com/api/character/7', 'created': '2017-11-04T19:59:20.523Z'}, {'id': 8, 'name': 'Adjudicator Rick', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/8.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/8', 'created': '2017-11-04T20:03:34.737Z'}, {'id': 9, 'name': 'Agency Director', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/9.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/24'], 'url': 'https://rickandmortyapi.com/api/character/9', 'created': '2017-11-04T20:06:54.976Z'}, {'id': 10, 'name': 'Alan Rails', 'status': 'Dead', 'species': 'Human', 'type': 'Superhuman (Ghost trains summoner)', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': "Worldender's lair", 'url': 'https://rickandmortyapi.com/api/location/4'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/10.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/25'], 'url': 'https://rickandmortyapi.com/api/character/10', 'created': '2017-11-04T20:19:09.017Z'}, {'id': 11, 'name': 'Albert Einstein', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/11.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/12'], 'url': 'https://rickandmortyapi.com/api/character/11', 'created': '2017-11-04T20:20:20.965Z'}, {'id': 12, 'name': 'Alexander', 'status': 'Dead', 'species': 'Human', 'type': '', 'gender': 'Male', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/12.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/12', 'created': '2017-11-04T20:32:33.144Z'}, {'id': 13, 'name': 'Alien Googah', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'unknown', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/13.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/31'], 'url': 'https://rickandmortyapi.com/api/character/13', 'created': '2017-11-04T20:33:30.779Z'}, {'id': 14, 'name': 'Alien Morty', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/14.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/14', 'created': '2017-11-04T20:51:31.373Z'}, {'id': 15, 'name': 'Alien Rick', 'status': 'unknown', 'species': 'Alien', 'type': '', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/15.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/15', 'created': '2017-11-04T20:56:13.215Z'}, {'id': 16, 'name': 'Amish Cyborg', 'status': 'Dead', 'species': 'Alien', 'type': 'Parasite', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Earth (Replacement Dimension)', 'url': 'https://rickandmortyapi.com/api/location/20'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/16.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/15'], 'url': 'https://rickandmortyapi.com/api/character/16', 'created': '2017-11-04T21:12:45.235Z'}, {'id': 17, 'name': 'Annie', 'status': 'Alive', 'species': 'Human', 'type': '', 'gender': 'Female', 'origin': {'name': 'Earth (C-137)', 'url': 'https://rickandmortyapi.com/api/location/1'}, 'location': {'name': 'Anatomy Park', 'url': 'https://rickandmortyapi.com/api/location/5'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/17.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/3'], 'url': 'https://rickandmortyapi.com/api/character/17', 'created': '2017-11-04T22:21:24.481Z'}, {'id': 18, 'name': 'Antenna Morty', 'status': 'Alive', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Citadel of Ricks', 'url': 'https://rickandmortyapi.com/api/location/3'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/18.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10', 'https://rickandmortyapi.com/api/episode/28'], 'url': 'https://rickandmortyapi.com/api/character/18', 'created': '2017-11-04T22:25:29.008Z'}, {'id': 19, 'name': 'Antenna Rick', 'status': 'unknown', 'species': 'Human', 'type': 'Human with antennae', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'unknown', 'url': ''}, 'image': 'https://rickandmortyapi.com/api/character/avatar/19.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/10'], 'url': 'https://rickandmortyapi.com/api/character/19', 'created': '2017-11-04T22:28:13.756Z'}, {'id': 20, 'name': 'Ants in my Eyes Johnson', 'status': 'unknown', 'species': 'Human', 'type': 'Human with ants in his eyes', 'gender': 'Male', 'origin': {'name': 'unknown', 'url': ''}, 'location': {'name': 'Interdimensional Cable', 'url': 'https://rickandmortyapi.com/api/location/6'}, 'image': 'https://rickandmortyapi.com/api/character/avatar/20.jpeg', 'episode': ['https://rickandmortyapi.com/api/episode/8'], 'url': 'https://rickandmortyapi.com/api/character/20', 'created': '2017-11-04T22:34:53.659Z'}]</t>
         </is>
       </c>
     </row>

</xml_diff>